<commit_message>
add extension ECLAIREArmIntervention 616ee09e3f73d1dfb6361f4438c5b269deafa6f2
</commit_message>
<xml_diff>
--- a/ig/sd-add-ext-intervention/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-add-ext-intervention/StructureDefinition-eclaire-researchstudy.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$109</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4077" uniqueCount="661">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-15T16:46:08+00:00</t>
+    <t>2024-02-15T17:22:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1933,6 +1933,22 @@
   </si>
   <si>
     <t>ResearchStudy.arm.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.arm.extension:eclaire-arm-intervention</t>
+  </si>
+  <si>
+    <t>eclaire-arm-intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/eclaire/StructureDefinition/eclaire-arm-intervention}
+</t>
+  </si>
+  <si>
+    <t>Intervention / For each arm of the trial record a brief intervention name plus an intervention description.</t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre du projet ECLAIRE pour indiquer les 'Interventions' dans les cohortes</t>
   </si>
   <si>
     <t>ResearchStudy.arm.modifierExtension</t>
@@ -2363,7 +2379,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO108"/>
+  <dimension ref="A1:AO109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -13901,11 +13917,13 @@
         <v>619</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>619</v>
-      </c>
-      <c r="C99" s="2"/>
+        <v>618</v>
+      </c>
+      <c r="C99" t="s" s="2">
+        <v>620</v>
+      </c>
       <c r="D99" t="s" s="2">
-        <v>620</v>
+        <v>80</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" t="s" s="2">
@@ -13915,29 +13933,25 @@
         <v>79</v>
       </c>
       <c r="H99" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I99" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J99" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K99" t="s" s="2">
-        <v>138</v>
+        <v>621</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="M99" t="s" s="2">
-        <v>622</v>
-      </c>
-      <c r="N99" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O99" t="s" s="2">
-        <v>214</v>
-      </c>
+        <v>623</v>
+      </c>
+      <c r="N99" s="2"/>
+      <c r="O99" s="2"/>
       <c r="P99" t="s" s="2">
         <v>80</v>
       </c>
@@ -13985,7 +13999,7 @@
         <v>80</v>
       </c>
       <c r="AF99" t="s" s="2">
-        <v>623</v>
+        <v>187</v>
       </c>
       <c r="AG99" t="s" s="2">
         <v>78</v>
@@ -14006,7 +14020,7 @@
         <v>80</v>
       </c>
       <c r="AM99" t="s" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="AN99" t="s" s="2">
         <v>80</v>
@@ -14024,37 +14038,39 @@
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
-        <v>80</v>
+        <v>625</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G100" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H100" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I100" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="O100" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="O100" t="s" s="2">
+        <v>214</v>
+      </c>
       <c r="P100" t="s" s="2">
         <v>80</v>
       </c>
@@ -14102,31 +14118,31 @@
         <v>80</v>
       </c>
       <c r="AF100" t="s" s="2">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="AG100" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH100" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI100" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK100" t="s" s="2">
-        <v>627</v>
+        <v>80</v>
       </c>
       <c r="AL100" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM100" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN100" t="s" s="2">
-        <v>628</v>
+        <v>80</v>
       </c>
       <c r="AO100" t="s" s="2">
         <v>80</v>
@@ -14145,7 +14161,7 @@
       </c>
       <c r="E101" s="2"/>
       <c r="F101" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G101" t="s" s="2">
         <v>90</v>
@@ -14160,7 +14176,7 @@
         <v>80</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>250</v>
+        <v>179</v>
       </c>
       <c r="L101" t="s" s="2">
         <v>630</v>
@@ -14169,7 +14185,7 @@
         <v>631</v>
       </c>
       <c r="N101" t="s" s="2">
-        <v>367</v>
+        <v>337</v>
       </c>
       <c r="O101" s="2"/>
       <c r="P101" t="s" s="2">
@@ -14222,7 +14238,7 @@
         <v>629</v>
       </c>
       <c r="AG101" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH101" t="s" s="2">
         <v>90</v>
@@ -14237,10 +14253,10 @@
         <v>632</v>
       </c>
       <c r="AL101" t="s" s="2">
-        <v>371</v>
+        <v>80</v>
       </c>
       <c r="AM101" t="s" s="2">
-        <v>372</v>
+        <v>111</v>
       </c>
       <c r="AN101" t="s" s="2">
         <v>633</v>
@@ -14277,7 +14293,7 @@
         <v>80</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>179</v>
+        <v>250</v>
       </c>
       <c r="L102" t="s" s="2">
         <v>635</v>
@@ -14286,7 +14302,7 @@
         <v>636</v>
       </c>
       <c r="N102" t="s" s="2">
-        <v>337</v>
+        <v>367</v>
       </c>
       <c r="O102" s="2"/>
       <c r="P102" t="s" s="2">
@@ -14354,10 +14370,10 @@
         <v>637</v>
       </c>
       <c r="AL102" t="s" s="2">
-        <v>80</v>
+        <v>371</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>111</v>
+        <v>372</v>
       </c>
       <c r="AN102" t="s" s="2">
         <v>638</v>
@@ -14382,7 +14398,7 @@
         <v>78</v>
       </c>
       <c r="G103" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H103" t="s" s="2">
         <v>80</v>
@@ -14394,7 +14410,7 @@
         <v>80</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>612</v>
+        <v>179</v>
       </c>
       <c r="L103" t="s" s="2">
         <v>640</v>
@@ -14402,7 +14418,9 @@
       <c r="M103" t="s" s="2">
         <v>641</v>
       </c>
-      <c r="N103" s="2"/>
+      <c r="N103" t="s" s="2">
+        <v>337</v>
+      </c>
       <c r="O103" s="2"/>
       <c r="P103" t="s" s="2">
         <v>80</v>
@@ -14457,7 +14475,7 @@
         <v>78</v>
       </c>
       <c r="AH103" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI103" t="s" s="2">
         <v>102</v>
@@ -14475,7 +14493,7 @@
         <v>111</v>
       </c>
       <c r="AN103" t="s" s="2">
-        <v>80</v>
+        <v>643</v>
       </c>
       <c r="AO103" t="s" s="2">
         <v>80</v>
@@ -14483,10 +14501,10 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B104" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
@@ -14497,7 +14515,7 @@
         <v>78</v>
       </c>
       <c r="G104" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H104" t="s" s="2">
         <v>80</v>
@@ -14509,13 +14527,13 @@
         <v>80</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>179</v>
+        <v>612</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>180</v>
+        <v>645</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>181</v>
+        <v>646</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -14566,22 +14584,22 @@
         <v>80</v>
       </c>
       <c r="AF104" t="s" s="2">
-        <v>182</v>
+        <v>644</v>
       </c>
       <c r="AG104" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI104" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ104" t="s" s="2">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="AK104" t="s" s="2">
-        <v>80</v>
+        <v>647</v>
       </c>
       <c r="AL104" t="s" s="2">
         <v>80</v>
@@ -14598,21 +14616,21 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" t="s" s="2">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G105" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H105" t="s" s="2">
         <v>80</v>
@@ -14624,17 +14642,15 @@
         <v>80</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="M105" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N105" t="s" s="2">
-        <v>141</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="N105" s="2"/>
       <c r="O105" s="2"/>
       <c r="P105" t="s" s="2">
         <v>80</v>
@@ -14671,31 +14687,31 @@
         <v>80</v>
       </c>
       <c r="AB105" t="s" s="2">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="AC105" t="s" s="2">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="AD105" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="AF105" t="s" s="2">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="AG105" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH105" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI105" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ105" t="s" s="2">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="AK105" t="s" s="2">
         <v>80</v>
@@ -14704,7 +14720,7 @@
         <v>80</v>
       </c>
       <c r="AM105" t="s" s="2">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="AN105" t="s" s="2">
         <v>80</v>
@@ -14715,14 +14731,14 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" t="s" s="2">
-        <v>620</v>
+        <v>137</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" t="s" s="2">
@@ -14735,26 +14751,24 @@
         <v>80</v>
       </c>
       <c r="I106" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K106" t="s" s="2">
         <v>138</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>621</v>
+        <v>139</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>622</v>
+        <v>235</v>
       </c>
       <c r="N106" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="O106" t="s" s="2">
-        <v>214</v>
-      </c>
+      <c r="O106" s="2"/>
       <c r="P106" t="s" s="2">
         <v>80</v>
       </c>
@@ -14790,19 +14804,19 @@
         <v>80</v>
       </c>
       <c r="AB106" t="s" s="2">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AC106" t="s" s="2">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AD106" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="AF106" t="s" s="2">
-        <v>623</v>
+        <v>187</v>
       </c>
       <c r="AG106" t="s" s="2">
         <v>78</v>
@@ -14834,44 +14848,46 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="B107" t="s" s="2">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" t="s" s="2">
-        <v>80</v>
+        <v>625</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G107" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H107" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I107" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J107" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>647</v>
+        <v>626</v>
       </c>
       <c r="M107" t="s" s="2">
-        <v>648</v>
+        <v>627</v>
       </c>
       <c r="N107" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="O107" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="O107" t="s" s="2">
+        <v>214</v>
+      </c>
       <c r="P107" t="s" s="2">
         <v>80</v>
       </c>
@@ -14919,28 +14935,28 @@
         <v>80</v>
       </c>
       <c r="AF107" t="s" s="2">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="AG107" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH107" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI107" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ107" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>649</v>
+        <v>80</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM107" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN107" t="s" s="2">
         <v>80</v>
@@ -14951,10 +14967,10 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
@@ -14977,16 +14993,16 @@
         <v>80</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>250</v>
+        <v>179</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="N108" t="s" s="2">
-        <v>367</v>
+        <v>337</v>
       </c>
       <c r="O108" s="2"/>
       <c r="P108" t="s" s="2">
@@ -15012,13 +15028,13 @@
         <v>80</v>
       </c>
       <c r="X108" t="s" s="2">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="Y108" t="s" s="2">
-        <v>653</v>
+        <v>80</v>
       </c>
       <c r="Z108" t="s" s="2">
-        <v>654</v>
+        <v>80</v>
       </c>
       <c r="AA108" t="s" s="2">
         <v>80</v>
@@ -15036,7 +15052,7 @@
         <v>80</v>
       </c>
       <c r="AF108" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="AG108" t="s" s="2">
         <v>78</v>
@@ -15051,23 +15067,140 @@
         <v>103</v>
       </c>
       <c r="AK108" t="s" s="2">
+        <v>654</v>
+      </c>
+      <c r="AL108" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM108" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AN108" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO108" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="109" hidden="true">
+      <c r="A109" t="s" s="2">
         <v>655</v>
       </c>
-      <c r="AL108" t="s" s="2">
+      <c r="B109" t="s" s="2">
+        <v>655</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G109" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K109" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="L109" t="s" s="2">
+        <v>656</v>
+      </c>
+      <c r="M109" t="s" s="2">
+        <v>657</v>
+      </c>
+      <c r="N109" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="O109" s="2"/>
+      <c r="P109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q109" s="2"/>
+      <c r="R109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X109" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="Y109" t="s" s="2">
+        <v>658</v>
+      </c>
+      <c r="Z109" t="s" s="2">
+        <v>659</v>
+      </c>
+      <c r="AA109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF109" t="s" s="2">
+        <v>655</v>
+      </c>
+      <c r="AG109" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH109" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI109" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ109" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK109" t="s" s="2">
+        <v>660</v>
+      </c>
+      <c r="AL109" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="AM108" t="s" s="2">
+      <c r="AM109" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AN108" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AO108" t="s" s="2">
+      <c r="AN109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO109" t="s" s="2">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO108">
+  <autoFilter ref="A1:AO109">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -15077,7 +15210,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI107">
+  <conditionalFormatting sqref="A2:AI108">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>